<commit_message>
dallay shal entay 16/02/2021
</commit_message>
<xml_diff>
--- a/Daily_Sale_Entry.xlsx
+++ b/Daily_Sale_Entry.xlsx
@@ -10,19 +10,46 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$3:$J$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$3:$K$48</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>gro on</t>
   </si>
   <si>
     <t>Sl.no</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Mrp.rate</t>
+  </si>
+  <si>
+    <t>Shal.rate</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bisk Fram Googly </t>
+  </si>
+  <si>
+    <t>1 pkt.</t>
+  </si>
+  <si>
+    <t>1 pc.</t>
+  </si>
+  <si>
+    <t>kissam Mango jam</t>
+  </si>
+  <si>
+    <t>Nafice Rice</t>
   </si>
 </sst>
 </file>
@@ -53,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -165,16 +192,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -193,9 +260,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,297 +570,367 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:J49"/>
+  <dimension ref="B1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" zoomScaleSheetLayoutView="58" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleSheetLayoutView="58" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="6" max="6" width="0.140625" customWidth="1"/>
+    <col min="7" max="7" width="3.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5703125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" customHeight="1"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1"/>
-    <row r="3" spans="2:10">
-      <c r="B3" s="5" t="s">
+    <row r="1" spans="2:11" ht="15" customHeight="1"/>
+    <row r="2" spans="2:11" ht="15.75" thickBot="1"/>
+    <row r="3" spans="2:11">
+      <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="2:10">
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="2:10">
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="11" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="12"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="C7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="18">
+        <v>1</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="12"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="I8" s="1">
+        <v>22</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="18">
+        <v>2</v>
+      </c>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="12"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="18">
+        <v>3</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="21" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="12"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="I10" s="1">
+        <v>110</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="12"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="12"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="2:11">
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="B14" s="12"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="2:11">
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="2:10">
-      <c r="B15" s="12"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="2:11">
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="2:10">
-      <c r="B16" s="12"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="12"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="2:11">
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="12"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="2:11">
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="12"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="2:11">
+      <c r="B19" s="18"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="12"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="2:11">
+      <c r="B20" s="18"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="12"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="2:11">
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="2:10">
-      <c r="B22" s="12"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="2:11">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="2:10">
-      <c r="B23" s="12"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="2:11">
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="12"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="2:11">
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="12"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="2:11">
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="12"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="2:10">
-      <c r="B27" s="12"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="2:10">
-      <c r="B28" s="12"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" s="6"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -788,10 +938,11 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="12"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" s="6"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -799,10 +950,11 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="2:10">
-      <c r="B30" s="12"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="6"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -810,10 +962,11 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="2:10">
-      <c r="B31" s="12"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" s="6"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -821,10 +974,11 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="2:10">
-      <c r="B32" s="12"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" s="6"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -832,10 +986,11 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="2:10">
-      <c r="B33" s="12"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="6"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -843,10 +998,11 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="2:10">
-      <c r="B34" s="12"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34" s="6"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -854,10 +1010,11 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="2"/>
-    </row>
-    <row r="35" spans="2:10">
-      <c r="B35" s="12"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35" s="6"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -865,10 +1022,11 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="2"/>
-    </row>
-    <row r="36" spans="2:10">
-      <c r="B36" s="12"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="6"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -876,10 +1034,11 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="2"/>
-    </row>
-    <row r="37" spans="2:10">
-      <c r="B37" s="12"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="2"/>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" s="6"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -887,10 +1046,11 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="2:10">
-      <c r="B38" s="12"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="B38" s="6"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -898,10 +1058,11 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="2"/>
-    </row>
-    <row r="39" spans="2:10">
-      <c r="B39" s="12"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="B39" s="6"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -909,10 +1070,11 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="2"/>
-    </row>
-    <row r="40" spans="2:10">
-      <c r="B40" s="12"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="6"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -920,10 +1082,11 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="2"/>
-    </row>
-    <row r="41" spans="2:10">
-      <c r="B41" s="12"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="2"/>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="B41" s="6"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -931,10 +1094,11 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="2:10">
-      <c r="B42" s="12"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="2:11">
+      <c r="B42" s="6"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -942,10 +1106,11 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="2"/>
-    </row>
-    <row r="43" spans="2:10">
-      <c r="B43" s="12"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="2"/>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="B43" s="6"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -953,10 +1118,11 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="2"/>
-    </row>
-    <row r="44" spans="2:10">
-      <c r="B44" s="12"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="B44" s="6"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -964,10 +1130,11 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="2"/>
-    </row>
-    <row r="45" spans="2:10">
-      <c r="B45" s="12"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="2"/>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45" s="6"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -975,10 +1142,11 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="2"/>
-    </row>
-    <row r="46" spans="2:10">
-      <c r="B46" s="12"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="2"/>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="6"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -986,10 +1154,11 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="2:10">
-      <c r="B47" s="12"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="2"/>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="6"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -997,38 +1166,29 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="2:10">
-      <c r="B48" s="12"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="2"/>
-    </row>
-    <row r="49" spans="2:10" ht="15.75" thickBot="1">
-      <c r="B49" s="13"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="4"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="2"/>
+    </row>
+    <row r="48" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B48" s="7"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:J6"/>
+    <mergeCell ref="B3:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="99" orientation="portrait" r:id="rId1"/>
   <rowBreaks count="1" manualBreakCount="1">
-    <brk id="49" min="1" max="9" man="1"/>
+    <brk id="48" min="1" max="9" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
data push 12:00 jobe work
</commit_message>
<xml_diff>
--- a/Daily_Sale_Entry.xlsx
+++ b/Daily_Sale_Entry.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15255" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Dally Sheles" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="344">
   <si>
     <t>gro on</t>
   </si>
@@ -1038,6 +1038,21 @@
   </si>
   <si>
     <t>kissan Mango Jam</t>
+  </si>
+  <si>
+    <t>emami refinr Oil (500 )</t>
+  </si>
+  <si>
+    <t>Kakima</t>
+  </si>
+  <si>
+    <t>Mashal Kachi Ghabi (buttol)(500 )</t>
+  </si>
+  <si>
+    <t>Googly Biskut</t>
+  </si>
+  <si>
+    <t>jk Masterd (Sarsay) ( 50 gm. )</t>
   </si>
 </sst>
 </file>
@@ -1595,7 +1610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1798,6 +1813,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="8" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2151,8 +2167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScaleSheetLayoutView="58" workbookViewId="0">
-      <selection activeCell="O32" sqref="O32"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleSheetLayoutView="58" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2172,73 +2188,73 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:11">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="110"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="110"/>
+      <c r="G2" s="110"/>
+      <c r="H2" s="110"/>
+      <c r="I2" s="110"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="111"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="113"/>
+      <c r="A3" s="112"/>
+      <c r="B3" s="113"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+      <c r="J3" s="113"/>
+      <c r="K3" s="114"/>
     </row>
     <row r="4" spans="1:11" ht="9" customHeight="1">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
-      <c r="K4" s="113"/>
+      <c r="A4" s="112"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
+      <c r="K4" s="114"/>
     </row>
     <row r="5" spans="1:11" hidden="1">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
-      <c r="K5" s="113"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="113"/>
+      <c r="E5" s="113"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="113"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
+      <c r="K5" s="114"/>
     </row>
     <row r="6" spans="1:11" ht="23.25" customHeight="1" thickBot="1">
-      <c r="A6" s="114" t="s">
+      <c r="A6" s="115" t="s">
         <v>275</v>
       </c>
-      <c r="B6" s="115"/>
-      <c r="C6" s="115"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="115"/>
-      <c r="G6" s="115"/>
-      <c r="H6" s="115"/>
-      <c r="I6" s="115"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="116"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="116"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
+      <c r="I6" s="116"/>
+      <c r="J6" s="116"/>
+      <c r="K6" s="117"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1">
       <c r="A7" s="43" t="s">
@@ -2749,11 +2765,21 @@
       <c r="K28" s="42"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="6"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
+      <c r="A29" s="6">
+        <v>16</v>
+      </c>
+      <c r="B29" s="108">
+        <v>44229</v>
+      </c>
+      <c r="C29" s="36">
+        <v>1</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>339</v>
+      </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2762,43 +2788,71 @@
       <c r="K29" s="42"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="6"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="A30" s="6">
+        <v>17</v>
+      </c>
+      <c r="B30" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="C30" s="36">
+        <v>1</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>341</v>
+      </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-      <c r="I30" s="6"/>
+      <c r="I30" s="6">
+        <v>87</v>
+      </c>
       <c r="J30" s="1"/>
-      <c r="K30" s="42"/>
+      <c r="K30" s="42">
+        <v>75</v>
+      </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="6"/>
       <c r="B31" s="36"/>
       <c r="C31" s="36"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="6" t="s">
+        <v>342</v>
+      </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="6"/>
+      <c r="I31" s="6">
+        <v>22</v>
+      </c>
       <c r="J31" s="1"/>
-      <c r="K31" s="42"/>
+      <c r="K31" s="42">
+        <v>21</v>
+      </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="6"/>
       <c r="B32" s="36"/>
       <c r="C32" s="36"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="D32" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>343</v>
+      </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="6"/>
+      <c r="I32" s="6">
+        <v>11</v>
+      </c>
       <c r="J32" s="1"/>
-      <c r="K32" s="42"/>
+      <c r="K32" s="42">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="6"/>
@@ -3025,8 +3079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:J325"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J137" sqref="J137"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="F114" sqref="F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7763,11 +7817,11 @@
     <row r="3" spans="3:14" ht="15.75" thickBot="1"/>
     <row r="4" spans="3:14">
       <c r="C4" s="68"/>
-      <c r="D4" s="117" t="s">
+      <c r="D4" s="118" t="s">
         <v>327</v>
       </c>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="E4" s="119"/>
+      <c r="F4" s="119"/>
       <c r="G4" s="69"/>
       <c r="H4" s="69"/>
       <c r="I4" s="69" t="s">
@@ -7781,9 +7835,9 @@
     </row>
     <row r="5" spans="3:14" ht="17.25" customHeight="1">
       <c r="C5" s="70"/>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
+      <c r="D5" s="120"/>
+      <c r="E5" s="120"/>
+      <c r="F5" s="120"/>
       <c r="G5" s="65"/>
       <c r="H5" s="65"/>
       <c r="I5" s="65"/>
@@ -7793,9 +7847,9 @@
     </row>
     <row r="6" spans="3:14" ht="8.25" customHeight="1">
       <c r="C6" s="70"/>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
+      <c r="D6" s="120"/>
+      <c r="E6" s="120"/>
+      <c r="F6" s="120"/>
       <c r="G6" s="65"/>
       <c r="H6" s="65"/>
       <c r="I6" s="65"/>
@@ -8022,8 +8076,8 @@
       <c r="H20" s="1"/>
       <c r="I20" s="6"/>
       <c r="J20" s="80"/>
-      <c r="K20" s="120"/>
-      <c r="L20" s="121"/>
+      <c r="K20" s="121"/>
+      <c r="L20" s="122"/>
       <c r="M20" s="78"/>
       <c r="N20" s="1"/>
     </row>
@@ -8084,26 +8138,26 @@
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="3:14">
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="124" t="s">
         <v>328</v>
       </c>
-      <c r="D25" s="124"/>
-      <c r="E25" s="124"/>
+      <c r="D25" s="125"/>
+      <c r="E25" s="125"/>
       <c r="F25" s="67"/>
       <c r="G25" s="67"/>
       <c r="H25" s="67"/>
       <c r="I25" s="67"/>
-      <c r="J25" s="122" t="s">
+      <c r="J25" s="123" t="s">
         <v>320</v>
       </c>
-      <c r="K25" s="122"/>
+      <c r="K25" s="123"/>
       <c r="L25" s="2"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="3:14" ht="15.75" thickBot="1">
-      <c r="C26" s="125"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="126"/>
+      <c r="C26" s="126"/>
+      <c r="D26" s="127"/>
+      <c r="E26" s="127"/>
       <c r="F26" s="72"/>
       <c r="G26" s="73"/>
       <c r="H26" s="73"/>
@@ -8129,8 +8183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8651,5 +8705,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>